<commit_message>
Readme and data updated
Co-Authored-By: Roberto Bastone <robertobastone@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22725"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22729"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67B2E7BD-7B50-4BEF-B6F4-B02213AC72FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A7FFB86-1BE6-405B-ABC9-844B0BB11A4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="activeCases" sheetId="1" r:id="rId1"/>
+    <sheet name="totalCases" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Region</t>
   </si>
@@ -92,6 +93,15 @@
   <si>
     <t>Italia</t>
   </si>
+  <si>
+    <t>Cured</t>
+  </si>
+  <si>
+    <t>Deceased</t>
+  </si>
+  <si>
+    <t>Total number of cases</t>
+  </si>
 </sst>
 </file>
 
@@ -137,13 +147,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -460,20 +471,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:AA1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.5703125" hidden="1" customWidth="1"/>
     <col min="5" max="9" width="10.5703125" style="1" hidden="1" customWidth="1"/>
     <col min="10" max="18" width="10.5703125" hidden="1" customWidth="1"/>
     <col min="19" max="20" width="10.85546875" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" hidden="1" customWidth="1"/>
+    <col min="23" max="26" width="10.5703125" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="10.85546875" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
@@ -546,6 +559,21 @@
       <c r="W1" s="5">
         <v>43917</v>
       </c>
+      <c r="X1" s="5">
+        <v>43918</v>
+      </c>
+      <c r="Y1" s="5">
+        <v>43919</v>
+      </c>
+      <c r="Z1" s="5">
+        <v>43920</v>
+      </c>
+      <c r="AA1" s="5">
+        <v>43921</v>
+      </c>
+      <c r="AB1" s="5">
+        <v>43922</v>
+      </c>
     </row>
     <row r="2" spans="1:34">
       <c r="A2" s="4" t="s">
@@ -617,11 +645,21 @@
       <c r="W2" s="2">
         <v>925</v>
       </c>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
+      <c r="X2" s="2">
+        <v>1027</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>1169</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>1169</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>1191</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>1211</v>
+      </c>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
@@ -699,11 +737,21 @@
       <c r="W3" s="2">
         <v>147</v>
       </c>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
+      <c r="X3" s="2">
+        <v>178</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>197</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>208</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>216</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>225</v>
+      </c>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
@@ -781,11 +829,21 @@
       <c r="W4" s="2">
         <v>469</v>
       </c>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
+      <c r="X4" s="2">
+        <v>523</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>577</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>602</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>606</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>610</v>
+      </c>
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
@@ -863,11 +921,21 @@
       <c r="W5" s="2">
         <v>1292</v>
       </c>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="2"/>
+      <c r="X5" s="2">
+        <v>1407</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>1556</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>1739</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>1871</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>1976</v>
+      </c>
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
@@ -945,11 +1013,21 @@
       <c r="W6" s="2">
         <v>9361</v>
       </c>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-      <c r="AA6" s="2"/>
-      <c r="AB6" s="2"/>
+      <c r="X6" s="2">
+        <v>9964</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>10535</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>10766</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>10953</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>11489</v>
+      </c>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
@@ -1027,11 +1105,21 @@
       <c r="W7" s="2">
         <v>1027</v>
       </c>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="2"/>
+      <c r="X7" s="2">
+        <v>1120</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>1141</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>1109</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>1160</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>1206</v>
+      </c>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
       <c r="AE7" s="2"/>
@@ -1109,11 +1197,21 @@
       <c r="W8" s="2">
         <v>2013</v>
       </c>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-      <c r="AA8" s="2"/>
-      <c r="AB8" s="2"/>
+      <c r="X8" s="2">
+        <v>2181</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>2362</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>2497</v>
+      </c>
+      <c r="AA8" s="2">
+        <v>2642</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>2758</v>
+      </c>
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
       <c r="AE8" s="2"/>
@@ -1191,11 +1289,21 @@
       <c r="W9" s="2">
         <v>2060</v>
       </c>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
-      <c r="AA9" s="2"/>
-      <c r="AB9" s="2"/>
+      <c r="X9" s="2">
+        <v>2086</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>2279</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>2383</v>
+      </c>
+      <c r="AA9" s="2">
+        <v>2508</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>2645</v>
+      </c>
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
       <c r="AE9" s="2"/>
@@ -1273,11 +1381,21 @@
       <c r="W10" s="2">
         <v>23895</v>
       </c>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
-      <c r="AA10" s="2"/>
-      <c r="AB10" s="2"/>
+      <c r="X10" s="2">
+        <v>24509</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>25392</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>25006</v>
+      </c>
+      <c r="AA10" s="2">
+        <v>25124</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>25765</v>
+      </c>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
       <c r="AE10" s="2"/>
@@ -1355,11 +1473,21 @@
       <c r="W11" s="2">
         <v>2850</v>
       </c>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="2"/>
-      <c r="Z11" s="2"/>
-      <c r="AA11" s="2"/>
-      <c r="AB11" s="2"/>
+      <c r="X11" s="2">
+        <v>2999</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>3160</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>3251</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>3352</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>3456</v>
+      </c>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
       <c r="AE11" s="2"/>
@@ -1437,11 +1565,21 @@
       <c r="W12" s="2">
         <v>86</v>
       </c>
-      <c r="X12" s="2"/>
-      <c r="Y12" s="2"/>
-      <c r="Z12" s="2"/>
-      <c r="AA12" s="2"/>
-      <c r="AB12" s="2"/>
+      <c r="X12" s="2">
+        <v>98</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>100</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>107</v>
+      </c>
+      <c r="AA12" s="2">
+        <v>117</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>131</v>
+      </c>
       <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
       <c r="AE12" s="2"/>
@@ -1519,11 +1657,21 @@
       <c r="W13" s="2">
         <v>6347</v>
       </c>
-      <c r="X13" s="2"/>
-      <c r="Y13" s="2"/>
-      <c r="Z13" s="2"/>
-      <c r="AA13" s="2"/>
-      <c r="AB13" s="2"/>
+      <c r="X13" s="2">
+        <v>6851</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>7268</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>7655</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>8082</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>8470</v>
+      </c>
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
       <c r="AE13" s="2"/>
@@ -1601,11 +1749,21 @@
       <c r="W14" s="2">
         <v>1236</v>
       </c>
-      <c r="X14" s="2"/>
-      <c r="Y14" s="2"/>
-      <c r="Z14" s="2"/>
-      <c r="AA14" s="2"/>
-      <c r="AB14" s="2"/>
+      <c r="X14" s="2">
+        <v>1358</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>1432</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>1585</v>
+      </c>
+      <c r="AA14" s="2">
+        <v>1654</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>1756</v>
+      </c>
       <c r="AC14" s="2"/>
       <c r="AD14" s="2"/>
       <c r="AE14" s="2"/>
@@ -1683,11 +1841,21 @@
       <c r="W15" s="2">
         <v>496</v>
       </c>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="2"/>
-      <c r="Z15" s="2"/>
-      <c r="AA15" s="2"/>
-      <c r="AB15" s="2"/>
+      <c r="X15" s="2">
+        <v>569</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>582</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>622</v>
+      </c>
+      <c r="AA15" s="2">
+        <v>657</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>675</v>
+      </c>
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
       <c r="AE15" s="2"/>
@@ -1765,11 +1933,21 @@
       <c r="W16" s="2">
         <v>1158</v>
       </c>
-      <c r="X16" s="2"/>
-      <c r="Y16" s="2"/>
-      <c r="Z16" s="2"/>
-      <c r="AA16" s="2"/>
-      <c r="AB16" s="2"/>
+      <c r="X16" s="2">
+        <v>1242</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>1330</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>1408</v>
+      </c>
+      <c r="AA16" s="2">
+        <v>1492</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>1544</v>
+      </c>
       <c r="AC16" s="2"/>
       <c r="AD16" s="2"/>
       <c r="AE16" s="2"/>
@@ -1847,11 +2025,21 @@
       <c r="W17" s="2">
         <v>3170</v>
       </c>
-      <c r="X17" s="2"/>
-      <c r="Y17" s="2"/>
-      <c r="Z17" s="2"/>
-      <c r="AA17" s="2"/>
-      <c r="AB17" s="2"/>
+      <c r="X17" s="2">
+        <v>3511</v>
+      </c>
+      <c r="Y17" s="2">
+        <v>3786</v>
+      </c>
+      <c r="Z17" s="2">
+        <v>4050</v>
+      </c>
+      <c r="AA17" s="2">
+        <v>4226</v>
+      </c>
+      <c r="AB17" s="2">
+        <v>4432</v>
+      </c>
       <c r="AC17" s="2"/>
       <c r="AD17" s="2"/>
       <c r="AE17" s="2"/>
@@ -1929,11 +2117,21 @@
       <c r="W18" s="2">
         <v>1997</v>
       </c>
-      <c r="X18" s="2"/>
-      <c r="Y18" s="2"/>
-      <c r="Z18" s="2"/>
-      <c r="AA18" s="2"/>
-      <c r="AB18" s="2"/>
+      <c r="X18" s="2">
+        <v>2163</v>
+      </c>
+      <c r="Y18" s="2">
+        <v>2327</v>
+      </c>
+      <c r="Z18" s="2">
+        <v>2455</v>
+      </c>
+      <c r="AA18" s="2">
+        <v>2531</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>2595</v>
+      </c>
       <c r="AC18" s="2"/>
       <c r="AD18" s="2"/>
       <c r="AE18" s="2"/>
@@ -2011,11 +2209,21 @@
       <c r="W19" s="2">
         <v>824</v>
       </c>
-      <c r="X19" s="2"/>
-      <c r="Y19" s="2"/>
-      <c r="Z19" s="2"/>
-      <c r="AA19" s="2"/>
-      <c r="AB19" s="2"/>
+      <c r="X19" s="2">
+        <v>898</v>
+      </c>
+      <c r="Y19" s="2">
+        <v>897</v>
+      </c>
+      <c r="Z19" s="2">
+        <v>834</v>
+      </c>
+      <c r="AA19" s="2">
+        <v>851</v>
+      </c>
+      <c r="AB19" s="2">
+        <v>864</v>
+      </c>
       <c r="AC19" s="2"/>
       <c r="AD19" s="2"/>
       <c r="AE19" s="2"/>
@@ -2093,11 +2301,21 @@
       <c r="W20" s="2">
         <v>413</v>
       </c>
-      <c r="X20" s="2"/>
-      <c r="Y20" s="2"/>
-      <c r="Z20" s="2"/>
-      <c r="AA20" s="2"/>
-      <c r="AB20" s="2"/>
+      <c r="X20" s="2">
+        <v>468</v>
+      </c>
+      <c r="Y20" s="2">
+        <v>539</v>
+      </c>
+      <c r="Z20" s="2">
+        <v>518</v>
+      </c>
+      <c r="AA20" s="2">
+        <v>552</v>
+      </c>
+      <c r="AB20" s="2">
+        <v>540</v>
+      </c>
       <c r="AC20" s="2"/>
       <c r="AD20" s="2"/>
       <c r="AE20" s="2"/>
@@ -2175,11 +2393,21 @@
       <c r="W21" s="2">
         <v>6648</v>
       </c>
-      <c r="X21" s="2"/>
-      <c r="Y21" s="2"/>
-      <c r="Z21" s="2"/>
-      <c r="AA21" s="2"/>
-      <c r="AB21" s="2"/>
+      <c r="X21" s="2">
+        <v>6913</v>
+      </c>
+      <c r="Y21" s="2">
+        <v>7251</v>
+      </c>
+      <c r="Z21" s="2">
+        <v>7564</v>
+      </c>
+      <c r="AA21" s="2">
+        <v>7850</v>
+      </c>
+      <c r="AB21" s="2">
+        <v>8224</v>
+      </c>
       <c r="AC21" s="2"/>
       <c r="AD21" s="2"/>
       <c r="AE21" s="2"/>
@@ -2279,6 +2507,446 @@
         <f>SUM(W2:W21)</f>
         <v>66414</v>
       </c>
+      <c r="X22" s="3">
+        <f t="shared" ref="X22:AB22" si="1">SUM(X2:X21)</f>
+        <v>70065</v>
+      </c>
+      <c r="Y22" s="3">
+        <f t="shared" si="1"/>
+        <v>73880</v>
+      </c>
+      <c r="Z22" s="3">
+        <f t="shared" si="1"/>
+        <v>75528</v>
+      </c>
+      <c r="AA22" s="3">
+        <f t="shared" si="1"/>
+        <v>77635</v>
+      </c>
+      <c r="AB22" s="3">
+        <f t="shared" si="1"/>
+        <v>80572</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{370018BD-AF2C-484B-9235-3FE7A6C4791B}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:AA1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="27" width="10.5703125" hidden="1" customWidth="1"/>
+    <col min="28" max="29" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29">
+      <c r="A1" t="str">
+        <f>activeCases!A1</f>
+        <v>Region</v>
+      </c>
+      <c r="B1" s="6">
+        <f>activeCases!B1</f>
+        <v>43896</v>
+      </c>
+      <c r="C1" s="6">
+        <f>activeCases!C1</f>
+        <v>43897</v>
+      </c>
+      <c r="D1" s="6">
+        <f>activeCases!D1</f>
+        <v>43898</v>
+      </c>
+      <c r="E1" s="6">
+        <f>activeCases!E1</f>
+        <v>43899</v>
+      </c>
+      <c r="F1" s="6">
+        <f>activeCases!F1</f>
+        <v>43900</v>
+      </c>
+      <c r="G1" s="6">
+        <f>activeCases!G1</f>
+        <v>43901</v>
+      </c>
+      <c r="H1" s="6">
+        <f>activeCases!H1</f>
+        <v>43902</v>
+      </c>
+      <c r="I1" s="6">
+        <f>activeCases!I1</f>
+        <v>43903</v>
+      </c>
+      <c r="J1" s="6">
+        <f>activeCases!J1</f>
+        <v>43904</v>
+      </c>
+      <c r="K1" s="6">
+        <f>activeCases!K1</f>
+        <v>43905</v>
+      </c>
+      <c r="L1" s="6">
+        <f>activeCases!L1</f>
+        <v>43906</v>
+      </c>
+      <c r="M1" s="6">
+        <f>activeCases!M1</f>
+        <v>43907</v>
+      </c>
+      <c r="N1" s="6">
+        <f>activeCases!N1</f>
+        <v>43908</v>
+      </c>
+      <c r="O1" s="6">
+        <f>activeCases!O1</f>
+        <v>43909</v>
+      </c>
+      <c r="P1" s="6">
+        <f>activeCases!P1</f>
+        <v>43910</v>
+      </c>
+      <c r="Q1" s="6">
+        <f>activeCases!Q1</f>
+        <v>43911</v>
+      </c>
+      <c r="R1" s="6">
+        <f>activeCases!R1</f>
+        <v>43912</v>
+      </c>
+      <c r="S1" s="6">
+        <f>activeCases!S1</f>
+        <v>43913</v>
+      </c>
+      <c r="T1" s="6">
+        <f>activeCases!T1</f>
+        <v>43914</v>
+      </c>
+      <c r="U1" s="6">
+        <f>activeCases!U1</f>
+        <v>43915</v>
+      </c>
+      <c r="V1" s="6">
+        <f>activeCases!V1</f>
+        <v>43916</v>
+      </c>
+      <c r="W1" s="6">
+        <f>activeCases!W1</f>
+        <v>43917</v>
+      </c>
+      <c r="X1" s="6">
+        <f>activeCases!X1</f>
+        <v>43918</v>
+      </c>
+      <c r="Y1" s="6">
+        <f>activeCases!Y1</f>
+        <v>43919</v>
+      </c>
+      <c r="Z1" s="6">
+        <f>activeCases!Z1</f>
+        <v>43920</v>
+      </c>
+      <c r="AA1" s="6">
+        <f>activeCases!AA1</f>
+        <v>43921</v>
+      </c>
+      <c r="AB1" s="6">
+        <f>activeCases!AB1</f>
+        <v>43922</v>
+      </c>
+      <c r="AC1" s="6"/>
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>523</v>
+      </c>
+      <c r="C2">
+        <v>589</v>
+      </c>
+      <c r="D2">
+        <v>622</v>
+      </c>
+      <c r="E2">
+        <v>724</v>
+      </c>
+      <c r="F2">
+        <v>1004</v>
+      </c>
+      <c r="G2">
+        <v>1045</v>
+      </c>
+      <c r="H2">
+        <v>1258</v>
+      </c>
+      <c r="I2">
+        <v>1439</v>
+      </c>
+      <c r="J2">
+        <v>1966</v>
+      </c>
+      <c r="K2">
+        <v>2335</v>
+      </c>
+      <c r="L2">
+        <v>2749</v>
+      </c>
+      <c r="M2">
+        <v>2941</v>
+      </c>
+      <c r="N2">
+        <v>4025</v>
+      </c>
+      <c r="O2">
+        <v>4440</v>
+      </c>
+      <c r="P2">
+        <v>5129</v>
+      </c>
+      <c r="Q2">
+        <v>6072</v>
+      </c>
+      <c r="R2">
+        <v>7024</v>
+      </c>
+      <c r="S2">
+        <v>7432</v>
+      </c>
+      <c r="T2">
+        <v>8326</v>
+      </c>
+      <c r="U2">
+        <v>9362</v>
+      </c>
+      <c r="V2">
+        <v>10361</v>
+      </c>
+      <c r="W2">
+        <v>10950</v>
+      </c>
+      <c r="X2">
+        <v>12384</v>
+      </c>
+      <c r="Y2">
+        <v>13030</v>
+      </c>
+      <c r="Z2">
+        <v>14620</v>
+      </c>
+      <c r="AA2">
+        <v>15729</v>
+      </c>
+      <c r="AB2">
+        <v>16847</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>197</v>
+      </c>
+      <c r="C3">
+        <v>233</v>
+      </c>
+      <c r="D3">
+        <v>366</v>
+      </c>
+      <c r="E3">
+        <v>463</v>
+      </c>
+      <c r="F3">
+        <v>631</v>
+      </c>
+      <c r="G3">
+        <v>827</v>
+      </c>
+      <c r="H3">
+        <v>1016</v>
+      </c>
+      <c r="I3">
+        <v>1266</v>
+      </c>
+      <c r="J3">
+        <v>1441</v>
+      </c>
+      <c r="K3">
+        <v>1809</v>
+      </c>
+      <c r="L3">
+        <v>2158</v>
+      </c>
+      <c r="M3">
+        <v>2503</v>
+      </c>
+      <c r="N3">
+        <v>2978</v>
+      </c>
+      <c r="O3">
+        <v>3405</v>
+      </c>
+      <c r="P3">
+        <v>4032</v>
+      </c>
+      <c r="Q3">
+        <v>4825</v>
+      </c>
+      <c r="R3">
+        <v>5476</v>
+      </c>
+      <c r="S3">
+        <v>6077</v>
+      </c>
+      <c r="T3">
+        <v>6820</v>
+      </c>
+      <c r="U3">
+        <v>7503</v>
+      </c>
+      <c r="V3">
+        <v>8165</v>
+      </c>
+      <c r="W3">
+        <v>9134</v>
+      </c>
+      <c r="X3">
+        <v>10023</v>
+      </c>
+      <c r="Y3">
+        <v>10779</v>
+      </c>
+      <c r="Z3">
+        <v>11591</v>
+      </c>
+      <c r="AA3">
+        <v>12428</v>
+      </c>
+      <c r="AB3">
+        <v>13155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2">
+        <f>SUM(activeCases!B22,B2:B3)</f>
+        <v>4636</v>
+      </c>
+      <c r="C4" s="2">
+        <f>SUM(activeCases!C22,C2:C3)</f>
+        <v>5883</v>
+      </c>
+      <c r="D4" s="2">
+        <f>SUM(activeCases!D22,D2:D3)</f>
+        <v>7375</v>
+      </c>
+      <c r="E4" s="2">
+        <f>SUM(activeCases!E22,E2:E3)</f>
+        <v>9172</v>
+      </c>
+      <c r="F4" s="2">
+        <f>SUM(activeCases!F22,F2:F3)</f>
+        <v>10149</v>
+      </c>
+      <c r="G4" s="2">
+        <f>SUM(activeCases!G22,G2:G3)</f>
+        <v>12462</v>
+      </c>
+      <c r="H4" s="2">
+        <f>SUM(activeCases!H22,H2:H3)</f>
+        <v>15113</v>
+      </c>
+      <c r="I4" s="2">
+        <f>SUM(activeCases!I22,I2:I3)</f>
+        <v>17660</v>
+      </c>
+      <c r="J4" s="2">
+        <f>SUM(activeCases!J22,J2:J3)</f>
+        <v>21157</v>
+      </c>
+      <c r="K4" s="2">
+        <f>SUM(activeCases!K22,K2:K3)</f>
+        <v>24747</v>
+      </c>
+      <c r="L4" s="2">
+        <f>SUM(activeCases!L22,L2:L3)</f>
+        <v>27980</v>
+      </c>
+      <c r="M4" s="2">
+        <f>SUM(activeCases!M22,M2:M3)</f>
+        <v>31506</v>
+      </c>
+      <c r="N4" s="2">
+        <f>SUM(activeCases!N22,N2:N3)</f>
+        <v>35713</v>
+      </c>
+      <c r="O4" s="2">
+        <f>SUM(activeCases!O22,O2:O3)</f>
+        <v>41035</v>
+      </c>
+      <c r="P4" s="2">
+        <f>SUM(activeCases!P22,P2:P3)</f>
+        <v>47021</v>
+      </c>
+      <c r="Q4" s="2">
+        <f>SUM(activeCases!Q22,Q2:Q3)</f>
+        <v>53564</v>
+      </c>
+      <c r="R4" s="2">
+        <f>SUM(activeCases!R22,R2:R3)</f>
+        <v>59138</v>
+      </c>
+      <c r="S4" s="2">
+        <f>SUM(activeCases!S22,S2:S3)</f>
+        <v>63927</v>
+      </c>
+      <c r="T4" s="2">
+        <f>SUM(activeCases!T22,T2:T3)</f>
+        <v>69176</v>
+      </c>
+      <c r="U4" s="2">
+        <f>SUM(activeCases!U22,U2:U3)</f>
+        <v>74386</v>
+      </c>
+      <c r="V4" s="2">
+        <f>SUM(activeCases!V22,V2:V3)</f>
+        <v>80539</v>
+      </c>
+      <c r="W4" s="2">
+        <f>SUM(activeCases!W22,W2:W3)</f>
+        <v>86498</v>
+      </c>
+      <c r="X4" s="2">
+        <f>SUM(activeCases!X22,X2:X3)</f>
+        <v>92472</v>
+      </c>
+      <c r="Y4" s="2">
+        <f>SUM(activeCases!Y22,Y2:Y3)</f>
+        <v>97689</v>
+      </c>
+      <c r="Z4" s="2">
+        <f>SUM(activeCases!Z22,Z2:Z3)</f>
+        <v>101739</v>
+      </c>
+      <c r="AA4" s="2">
+        <f>SUM(activeCases!AA22,AA2:AA3)</f>
+        <v>105792</v>
+      </c>
+      <c r="AB4" s="2">
+        <f>SUM(activeCases!AB22,AB2:AB3)</f>
+        <v>110574</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>